<commit_message>
commit excel json data changes
</commit_message>
<xml_diff>
--- a/excelFiles/lion-login.xlsx
+++ b/excelFiles/lion-login.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>password</t>
   </si>
@@ -40,6 +40,18 @@
   </si>
   <si>
     <t>userName</t>
+  </si>
+  <si>
+    <t>textbox</t>
+  </si>
+  <si>
+    <t>button</t>
+  </si>
+  <si>
+    <t>elementType</t>
+  </si>
+  <si>
+    <t>Locator</t>
   </si>
 </sst>
 </file>
@@ -381,20 +393,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -402,10 +416,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1">
+    <row r="2" spans="1:5" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -413,10 +433,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -424,15 +447,21 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>